<commit_message>
Updated the output folder
</commit_message>
<xml_diff>
--- a/output/structured_timetable.xlsx
+++ b/output/structured_timetable.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -34,10 +34,15 @@
     </font>
     <font>
       <b val="1"/>
+      <color rgb="00000000"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <b val="1"/>
       <sz val="12"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill/>
     </fill>
@@ -46,8 +51,32 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="009EB597"/>
-        <bgColor rgb="009EB597"/>
+        <fgColor rgb="0092A9C2"/>
+        <bgColor rgb="0092A9C2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00B990A5"/>
+        <bgColor rgb="00B990A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFD966"/>
+        <bgColor rgb="00FFD966"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00BE84C7"/>
+        <bgColor rgb="00BE84C7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0093A08C"/>
+        <bgColor rgb="0093A08C"/>
       </patternFill>
     </fill>
     <fill>
@@ -58,38 +87,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00B990A5"/>
-        <bgColor rgb="00B990A5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0092A9C2"/>
-        <bgColor rgb="0092A9C2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0093A08C"/>
-        <bgColor rgb="0093A08C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="00B5999C"/>
         <bgColor rgb="00B5999C"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00BE84C7"/>
-        <bgColor rgb="00BE84C7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="00A5C8A7"/>
         <bgColor rgb="00A5C8A7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="009EB597"/>
+        <bgColor rgb="009EB597"/>
       </patternFill>
     </fill>
   </fills>
@@ -111,12 +122,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -125,7 +136,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -141,6 +152,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -508,7 +522,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -526,6 +540,8 @@
     <col width="30" customWidth="1" min="9" max="9"/>
     <col width="30" customWidth="1" min="10" max="10"/>
     <col width="30" customWidth="1" min="11" max="11"/>
+    <col width="30" customWidth="1" min="12" max="12"/>
+    <col width="30" customWidth="1" min="13" max="13"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -536,14 +552,14 @@
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
+          <t>09:00 - 10:00</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
           <t>09:00 - 10:30</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
-        <is>
-          <t>09:00 - 11:00</t>
-        </is>
-      </c>
       <c r="D1" s="2" t="inlineStr">
         <is>
           <t>10:10 - 11:10</t>
@@ -561,136 +577,160 @@
       </c>
       <c r="G1" s="2" t="inlineStr">
         <is>
-          <t>14:10 - 15:10</t>
+          <t>13:00 - 14:00</t>
         </is>
       </c>
       <c r="H1" s="2" t="inlineStr">
         <is>
+          <t>14:00 - 15:30</t>
+        </is>
+      </c>
+      <c r="I1" s="2" t="inlineStr">
+        <is>
+          <t>14:00 - 16:00</t>
+        </is>
+      </c>
+      <c r="J1" s="2" t="inlineStr">
+        <is>
           <t>14:30 - 15:30</t>
         </is>
       </c>
-      <c r="I1" s="2" t="inlineStr">
-        <is>
-          <t>14:40 - 16:10</t>
-        </is>
-      </c>
-      <c r="J1" s="2" t="inlineStr">
+      <c r="K1" s="2" t="inlineStr">
+        <is>
+          <t>15:40 - 17:10</t>
+        </is>
+      </c>
+      <c r="L1" s="2" t="inlineStr">
         <is>
           <t>16:10 - 18:10</t>
         </is>
       </c>
-      <c r="K1" s="2" t="inlineStr">
-        <is>
-          <t>16:20 - 17:50</t>
+      <c r="M1" s="2" t="inlineStr">
+        <is>
+          <t>17:20 - 18:50</t>
         </is>
       </c>
     </row>
     <row r="2" ht="80" customHeight="1">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Tue</t>
-        </is>
-      </c>
-      <c r="B2" s="3" t="inlineStr">
-        <is>
-          <t>HS261
-HSS(Ethics &amp; Values) (Lecture)</t>
+          <t>Mon</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>MA261
+Differential Equations (Lecture)</t>
         </is>
       </c>
       <c r="E2" s="4" t="inlineStr">
+        <is>
+          <t>MA262
+Multivariate Calculus (Lecture)</t>
+        </is>
+      </c>
+      <c r="G2" s="5" t="inlineStr">
+        <is>
+          <t>Lunch Break</t>
+        </is>
+      </c>
+      <c r="H2" s="6" t="inlineStr">
+        <is>
+          <t>CS261
+Operating System (Lecture)</t>
+        </is>
+      </c>
+      <c r="K2" s="7" t="inlineStr">
+        <is>
+          <t>CS262
+Software Design Tools And Techniques (Lecture)</t>
+        </is>
+      </c>
+      <c r="M2" s="8" t="inlineStr">
         <is>
           <t>CS263
 Design &amp; Analysis of Algorithm (Lecture)</t>
-        </is>
-      </c>
-      <c r="G2" s="5" t="inlineStr">
-        <is>
-          <t>MA262
-Multivariate Calculus (Tutorial)</t>
-        </is>
-      </c>
-      <c r="K2" s="6" t="inlineStr">
-        <is>
-          <t>MA261
-Differential Equations (Lecture)</t>
         </is>
       </c>
     </row>
     <row r="3" ht="80" customHeight="1">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Thu</t>
-        </is>
-      </c>
-      <c r="B3" s="5" t="inlineStr">
+          <t>Tue</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>MA261
+Differential Equations (Lecture)</t>
+        </is>
+      </c>
+      <c r="E3" s="4" t="inlineStr">
         <is>
           <t>MA262
 Multivariate Calculus (Lecture)</t>
         </is>
       </c>
-      <c r="J3" s="7" t="inlineStr">
+      <c r="G3" s="5" t="inlineStr">
+        <is>
+          <t>Lunch Break</t>
+        </is>
+      </c>
+      <c r="H3" s="6" t="inlineStr">
+        <is>
+          <t>CS261
+Operating System (Lecture)</t>
+        </is>
+      </c>
+      <c r="K3" s="7" t="inlineStr">
         <is>
           <t>CS262
-Software Design Tools And Techniques (Lab)</t>
+Software Design Tools And Techniques (Lecture)</t>
+        </is>
+      </c>
+      <c r="M3" s="8" t="inlineStr">
+        <is>
+          <t>CS263
+Design &amp; Analysis of Algorithm (Lecture)</t>
         </is>
       </c>
     </row>
     <row r="4" ht="80" customHeight="1">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Fri</t>
-        </is>
-      </c>
-      <c r="E4" s="8" t="inlineStr">
-        <is>
-          <t>CS264
-Computer Networks (Lecture)</t>
-        </is>
-      </c>
-      <c r="F4" s="6" t="inlineStr">
+          <t>Wed</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
         <is>
           <t>MA261
 Differential Equations (Tutorial)</t>
         </is>
       </c>
-      <c r="I4" s="4" t="inlineStr">
-        <is>
-          <t>CS263
-Design &amp; Analysis of Algorithm (Lecture)
----
-HS261
-HSS(Ethics &amp; Values) (Lecture)</t>
-        </is>
-      </c>
-    </row>
-    <row r="5" ht="80" customHeight="1">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>Wed</t>
-        </is>
-      </c>
-      <c r="B5" s="7" t="inlineStr">
+      <c r="D4" s="4" t="inlineStr">
+        <is>
+          <t>MA262
+Multivariate Calculus (Tutorial)</t>
+        </is>
+      </c>
+      <c r="F4" s="9" t="inlineStr">
+        <is>
+          <t>CS264
+Computer Networks (Tutorial)</t>
+        </is>
+      </c>
+      <c r="G4" s="5" t="inlineStr">
+        <is>
+          <t>Lunch Break</t>
+        </is>
+      </c>
+      <c r="I4" s="7" t="inlineStr">
         <is>
           <t>CS262
-Software Design Tools And Techniques (Lecture)</t>
-        </is>
-      </c>
-      <c r="C5" s="4" t="inlineStr">
-        <is>
-          <t>CS263
-Design &amp; Analysis of Algorithm (Lab)</t>
-        </is>
-      </c>
-      <c r="E5" s="9" t="inlineStr">
-        <is>
-          <t>CS261
-Operating System (Lecture)
----
-CS264
-Computer Networks (Lecture)</t>
-        </is>
-      </c>
-      <c r="H5" s="10" t="inlineStr">
+Software Design Tools And Techniques (Lab)</t>
+        </is>
+      </c>
+      <c r="J4" s="10" t="inlineStr">
         <is>
           <t>EC251
 Open Elective - Electronics System Design - I
@@ -705,41 +745,58 @@
 Open Elective - 2D Computer Graphics</t>
         </is>
       </c>
+      <c r="L4" s="8" t="inlineStr">
+        <is>
+          <t>CS263
+Design &amp; Analysis of Algorithm (Lab)</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="80" customHeight="1">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Thu</t>
+        </is>
+      </c>
+      <c r="C5" s="9" t="inlineStr">
+        <is>
+          <t>CS264
+Computer Networks (Lecture)</t>
+        </is>
+      </c>
+      <c r="E5" s="11" t="inlineStr">
+        <is>
+          <t>HS261
+HSS(Ethics &amp; Values) (Lecture)</t>
+        </is>
+      </c>
+      <c r="G5" s="5" t="inlineStr">
+        <is>
+          <t>Lunch Break</t>
+        </is>
+      </c>
     </row>
     <row r="6" ht="80" customHeight="1">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Mon</t>
-        </is>
-      </c>
-      <c r="B6" s="5" t="inlineStr">
-        <is>
-          <t>MA262
-Multivariate Calculus (Lecture)</t>
-        </is>
-      </c>
-      <c r="D6" s="8" t="inlineStr">
+          <t>Fri</t>
+        </is>
+      </c>
+      <c r="C6" s="9" t="inlineStr">
         <is>
           <t>CS264
-Computer Networks (Tutorial)</t>
-        </is>
-      </c>
-      <c r="E6" s="6" t="inlineStr">
-        <is>
-          <t>MA261
-Differential Equations (Lecture)</t>
-        </is>
-      </c>
-      <c r="I6" s="9" t="inlineStr">
-        <is>
-          <t>CS261
-Operating System (Lecture)</t>
-        </is>
-      </c>
-      <c r="K6" s="7" t="inlineStr">
-        <is>
-          <t>CS262
-Software Design Tools And Techniques (Lecture)</t>
+Computer Networks (Lecture)</t>
+        </is>
+      </c>
+      <c r="E6" s="11" t="inlineStr">
+        <is>
+          <t>HS261
+HSS(Ethics &amp; Values) (Lecture)</t>
+        </is>
+      </c>
+      <c r="G6" s="5" t="inlineStr">
+        <is>
+          <t>Lunch Break</t>
         </is>
       </c>
     </row>

</xml_diff>